<commit_message>
[main] Fix valori report checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.1/report-checklist.xlsx
@@ -15,7 +15,8 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$52</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -787,7 +788,7 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">Il campo è presente staticamente nel template del CDA e non gestito da interfaccia</t>
+    <t xml:space="preserve">Campo valorizzato di default</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT6_KO</t>
@@ -1835,7 +1836,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2909,7 +2910,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -4019,7 +4020,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
-      <selection pane="bottomRight" activeCell="B35" activeCellId="0" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5800,7 +5801,7 @@
       <c r="J35" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K35" s="31" t="s">
+      <c r="K35" s="32" t="s">
         <v>173</v>
       </c>
       <c r="L35" s="32"/>
@@ -6880,7 +6881,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="92" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="27" t="n">
         <v>176</v>
       </c>
@@ -6896,16 +6897,14 @@
       <c r="E37" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="F37" s="30" t="n">
-        <v>45545</v>
-      </c>
+      <c r="F37" s="30"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
       <c r="I37" s="30"/>
       <c r="J37" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K37" s="31" t="s">
+      <c r="K37" s="32" t="s">
         <v>173</v>
       </c>
       <c r="L37" s="32"/>
@@ -7190,7 +7189,7 @@
       <c r="J42" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K42" s="31" t="s">
+      <c r="K42" s="32" t="s">
         <v>173</v>
       </c>
       <c r="L42" s="32"/>
@@ -7292,7 +7291,7 @@
       <c r="J44" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K44" s="31" t="s">
+      <c r="K44" s="32" t="s">
         <v>173</v>
       </c>
       <c r="L44" s="32"/>
@@ -7699,7 +7698,7 @@
       <c r="J51" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="K51" s="31" t="s">
+      <c r="K51" s="32" t="s">
         <v>173</v>
       </c>
       <c r="L51" s="32"/>
@@ -15307,7 +15306,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A9:W52"/>
+  <autoFilter ref="A9:W54"/>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -15317,7 +15316,7 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M10:N13 P10:P13 J37 M37:N37 P37 J42 M42:N42 P42 J44 M44:N44 P44 J51 M51:N52 P51:P52" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
@@ -15335,7 +15334,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M35:N35 P35:R35 M53:N54 P53:R54" type="list">
-      <formula1>#RIF!!$B$2:$B$3</formula1>
+      <formula1>#rif!!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K53:K54" type="list">
@@ -15343,11 +15342,15 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T35 T53:T54" type="list">
-      <formula1>#RIF!!$A$2:$A$3</formula1>
+      <formula1>#rif!!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J35" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K35 K37 K42 K44 K51" type="list">
+      <formula1>Summary!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -15376,7 +15379,7 @@
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -17057,7 +17060,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>

</xml_diff>

<commit_message>
[main] Fix test 444, 445
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.1/report-checklist.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$54</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$W$54</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="315">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1048,13 +1048,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-09-10T15:43:41Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b7242f70f13d5d92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.f2a3c05dcb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-09-17T10:33:43Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004c5769529253e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.45c38fad3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT2</t>
@@ -1065,10 +1065,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">71f38d5322e081f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.958832c656^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-09-17T10:33:45Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3fcca57d8ada8205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.9a95323c51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -1836,7 +1839,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2910,7 +2913,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -4016,11 +4019,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
-      <selection pane="bottomRight" activeCell="G37" activeCellId="0" sqref="G37"/>
+      <selection pane="bottomLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7780,7 +7783,7 @@
         <v>247</v>
       </c>
       <c r="F53" s="30" t="n">
-        <v>45545</v>
+        <v>45552</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>248</v>
@@ -8828,16 +8831,16 @@
         <v>252</v>
       </c>
       <c r="F54" s="30" t="n">
-        <v>45545</v>
+        <v>45552</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>176</v>
+        <v>253</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J54" s="31" t="s">
         <v>58</v>
@@ -15306,7 +15309,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A9:W54"/>
+  <autoFilter ref="A9:W52"/>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -15379,7 +15382,7 @@
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -15396,66 +15399,66 @@
         <v>29</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15463,41 +15466,41 @@
         <v>52</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15505,83 +15508,83 @@
         <v>75</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C11" s="54" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C12" s="54" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C13" s="54" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C14" s="54" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15589,41 +15592,41 @@
         <v>52</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C15" s="54" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C16" s="54" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C17" s="54" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="55" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15631,69 +15634,69 @@
         <v>75</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C18" s="54" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C19" s="54" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C20" s="54" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C21" s="54" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C22" s="54" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15701,41 +15704,41 @@
         <v>52</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C23" s="54" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C24" s="54" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C25" s="54" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15743,69 +15746,69 @@
         <v>75</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C26" s="54" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C27" s="54" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="54" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C28" s="54" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="54" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C29" s="54" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="56" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C30" s="54" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15813,41 +15816,41 @@
         <v>52</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C31" s="54" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C32" s="54" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="55" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C33" s="54" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15855,21 +15858,21 @@
         <v>75</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C34" s="54" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="55" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C35" s="54" t="n">
         <v>195</v>
@@ -15880,10 +15883,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C36" s="54" t="n">
         <v>211</v>
@@ -15894,10 +15897,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C37" s="54" t="n">
         <v>227</v>
@@ -15908,10 +15911,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C38" s="54" t="n">
         <v>243</v>
@@ -15925,7 +15928,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C39" s="54" t="n">
         <v>259</v>
@@ -15936,10 +15939,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C40" s="54" t="n">
         <v>275</v>
@@ -15950,10 +15953,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C41" s="54" t="n">
         <v>291</v>
@@ -15967,7 +15970,7 @@
         <v>75</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C42" s="54" t="n">
         <v>307</v>
@@ -15978,10 +15981,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C43" s="54" t="n">
         <v>196</v>
@@ -15992,10 +15995,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C44" s="54" t="n">
         <v>212</v>
@@ -16006,10 +16009,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C45" s="54" t="n">
         <v>228</v>
@@ -16020,10 +16023,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C46" s="54" t="n">
         <v>244</v>
@@ -16037,7 +16040,7 @@
         <v>52</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C47" s="54" t="n">
         <v>260</v>
@@ -16048,10 +16051,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C48" s="54" t="n">
         <v>276</v>
@@ -16062,10 +16065,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C49" s="54" t="n">
         <v>292</v>
@@ -16079,7 +16082,7 @@
         <v>75</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C50" s="54" t="n">
         <v>308</v>
@@ -17060,7 +17063,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -17077,7 +17080,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>58</v>
@@ -17085,7 +17088,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>82</v>

</xml_diff>